<commit_message>
Fix R4 to R7 PN
</commit_message>
<xml_diff>
--- a/P08R60/Released/BOM/P08R60.xlsx
+++ b/P08R60/Released/BOM/P08R60.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anas\Documents\Hexabitz\H08R60\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hexabitz_Github\Hardware\P08R6x-Hardware\P08R60\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5748A5EE-3C1F-4F8F-B332-5F66953FF1E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-30" windowWidth="23025" windowHeight="4335"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,8 +24,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="H10R4" type="6" refreshedVersion="4" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="H10R4" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="932" sourceFile="C:\Work\27\Asaad\Modules\H10R4\Delivery\Released\BOM\H10R4.csv" semicolon="1">
       <textFields count="14">
         <textField/>
@@ -44,7 +45,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="H10R41" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="H10R41" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="932" sourceFile="C:\Work\27\Asaad\Modules\H10R4\Delivery\Released\BOM\H10R4.csv" semicolon="1">
       <textFields count="14">
         <textField/>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
   <si>
     <t>Qty</t>
   </si>
@@ -281,17 +282,20 @@
   </si>
   <si>
     <t>https://octopart.com/erj-3geyj271v-panasonic-55560546</t>
+  </si>
+  <si>
+    <t>CRCW06032K20FKEA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -305,7 +309,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -382,7 +386,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="H10R4" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="H10R4" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -461,6 +465,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -496,6 +517,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -671,26 +709,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.25" customWidth="1"/>
-    <col min="2" max="2" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.375" customWidth="1"/>
-    <col min="4" max="4" width="60.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90.625" customWidth="1"/>
-    <col min="8" max="8" width="6.25" customWidth="1"/>
+    <col min="1" max="1" width="6.265625" customWidth="1"/>
+    <col min="2" max="2" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3984375" customWidth="1"/>
+    <col min="4" max="4" width="60.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90.59765625" customWidth="1"/>
+    <col min="8" max="8" width="6.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -716,7 +754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>6</v>
       </c>
@@ -739,7 +777,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -762,7 +800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -785,7 +823,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -808,7 +846,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -831,7 +869,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -854,7 +892,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -877,7 +915,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -900,7 +938,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -923,7 +961,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -937,16 +975,16 @@
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -969,7 +1007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -992,7 +1030,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>1</v>
       </c>

</xml_diff>